<commit_message>
2023-05-08 - Completed QCS - Improved project architecture
</commit_message>
<xml_diff>
--- a/output/fit_clients/fit_round_1.xlsx
+++ b/output/fit_clients/fit_round_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,25 +471,30 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>mu</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>isSelected</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>bandwidth</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>transRate</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>uploadTime</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>totalTime</t>
         </is>
@@ -522,19 +527,22 @@
       <c r="H2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="b">
+      <c r="I2" t="n">
+        <v>79684984</v>
+      </c>
+      <c r="J2" t="b">
         <v>0</v>
       </c>
-      <c r="J2" t="n">
-        <v>66666.66666666667</v>
-      </c>
       <c r="K2" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L2" t="n">
         <v>2285057.016324704</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>0.8683336940061932</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>487.0231240493583</v>
       </c>
     </row>
@@ -565,19 +573,22 @@
       <c r="H3" t="n">
         <v>20</v>
       </c>
-      <c r="I3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" t="n">
-        <v>66666.66666666667</v>
+      <c r="I3" t="n">
+        <v>79871352</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
       </c>
       <c r="K3" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L3" t="n">
         <v>2347839.027896418</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>0.8451141566454695</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>77.41631044958672</v>
       </c>
     </row>
@@ -608,19 +619,22 @@
       <c r="H4" t="n">
         <v>20</v>
       </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" t="n">
-        <v>66666.66666666667</v>
+      <c r="I4" t="n">
+        <v>79786872</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
       </c>
       <c r="K4" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L4" t="n">
         <v>2356476.436018003</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>0.8420164826060843</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>174.3540232399308</v>
       </c>
     </row>
@@ -651,19 +665,22 @@
       <c r="H5" t="n">
         <v>20</v>
       </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="n">
-        <v>66666.66666666667</v>
+      <c r="I5" t="n">
+        <v>79050104</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
       </c>
       <c r="K5" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L5" t="n">
         <v>2261945.303482444</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>0.8772060035869031</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>68.16556007597019</v>
       </c>
     </row>
@@ -694,19 +711,22 @@
       <c r="H6" t="n">
         <v>20</v>
       </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" t="n">
-        <v>66666.66666666667</v>
+      <c r="I6" t="n">
+        <v>79858040</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
       </c>
       <c r="K6" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L6" t="n">
         <v>2361316.125842037</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>0.8402907083406481</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>251.8743353326198</v>
       </c>
     </row>
@@ -737,19 +757,22 @@
       <c r="H7" t="n">
         <v>10</v>
       </c>
-      <c r="I7" t="b">
+      <c r="I7" t="n">
+        <v>79890808</v>
+      </c>
+      <c r="J7" t="b">
         <v>0</v>
       </c>
-      <c r="J7" t="n">
-        <v>66666.66666666667</v>
-      </c>
       <c r="K7" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L7" t="n">
         <v>2279183.352454564</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>0.8705714693217317</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
         <v>400.27882960734</v>
       </c>
     </row>
@@ -780,19 +803,22 @@
       <c r="H8" t="n">
         <v>0</v>
       </c>
-      <c r="I8" t="b">
+      <c r="I8" t="n">
+        <v>80089464</v>
+      </c>
+      <c r="J8" t="b">
         <v>0</v>
       </c>
-      <c r="J8" t="n">
-        <v>66666.66666666667</v>
-      </c>
       <c r="K8" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L8" t="n">
         <v>2287337.864454519</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>0.8674678239863735</v>
       </c>
-      <c r="M8" t="n">
+      <c r="N8" t="n">
         <v>750.051129148031</v>
       </c>
     </row>
@@ -823,19 +849,22 @@
       <c r="H9" t="n">
         <v>20</v>
       </c>
-      <c r="I9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" t="n">
-        <v>66666.66666666667</v>
+      <c r="I9" t="n">
+        <v>79675768</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
       </c>
       <c r="K9" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L9" t="n">
         <v>2351873.685337585</v>
       </c>
-      <c r="L9" t="n">
+      <c r="M9" t="n">
         <v>0.8436643567935459</v>
       </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
         <v>262.9795943153767</v>
       </c>
     </row>
@@ -866,19 +895,22 @@
       <c r="H10" t="n">
         <v>20</v>
       </c>
-      <c r="I10" t="b">
-        <v>1</v>
-      </c>
-      <c r="J10" t="n">
-        <v>66666.66666666667</v>
+      <c r="I10" t="n">
+        <v>80101240</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
       </c>
       <c r="K10" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L10" t="n">
         <v>2353131.690490548</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
         <v>0.8432133263167957</v>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>144.194968034549</v>
       </c>
     </row>
@@ -909,19 +941,22 @@
       <c r="H11" t="n">
         <v>20</v>
       </c>
-      <c r="I11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" t="n">
-        <v>66666.66666666667</v>
+      <c r="I11" t="n">
+        <v>79580024</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
       </c>
       <c r="K11" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L11" t="n">
         <v>2225689.479983788</v>
       </c>
-      <c r="L11" t="n">
+      <c r="M11" t="n">
         <v>0.8914954299979225</v>
       </c>
-      <c r="M11" t="n">
+      <c r="N11" t="n">
         <v>214.161864045828</v>
       </c>
     </row>
@@ -952,19 +987,22 @@
       <c r="H12" t="n">
         <v>20</v>
       </c>
-      <c r="I12" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" t="n">
-        <v>66666.66666666667</v>
+      <c r="I12" t="n">
+        <v>79984504</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
       </c>
       <c r="K12" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L12" t="n">
         <v>2301572.521061347</v>
       </c>
-      <c r="L12" t="n">
+      <c r="M12" t="n">
         <v>0.8621027501166939</v>
       </c>
-      <c r="M12" t="n">
+      <c r="N12" t="n">
         <v>195.3204204966414</v>
       </c>
     </row>
@@ -995,19 +1033,22 @@
       <c r="H13" t="n">
         <v>20</v>
       </c>
-      <c r="I13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" t="n">
-        <v>66666.66666666667</v>
+      <c r="I13" t="n">
+        <v>79686520</v>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
       </c>
       <c r="K13" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L13" t="n">
         <v>2329385.763906141</v>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="n">
         <v>0.8518091038183018</v>
       </c>
-      <c r="M13" t="n">
+      <c r="N13" t="n">
         <v>139.1077566148234</v>
       </c>
     </row>
@@ -1038,19 +1079,22 @@
       <c r="H14" t="n">
         <v>20</v>
       </c>
-      <c r="I14" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" t="n">
-        <v>66666.66666666667</v>
+      <c r="I14" t="n">
+        <v>79952248</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
       </c>
       <c r="K14" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L14" t="n">
         <v>2268737.726939628</v>
       </c>
-      <c r="L14" t="n">
+      <c r="M14" t="n">
         <v>0.8745797173640425</v>
       </c>
-      <c r="M14" t="n">
+      <c r="N14" t="n">
         <v>175.8864100908005</v>
       </c>
     </row>
@@ -1081,19 +1125,22 @@
       <c r="H15" t="n">
         <v>20</v>
       </c>
-      <c r="I15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" t="n">
-        <v>66666.66666666667</v>
+      <c r="I15" t="n">
+        <v>79846264</v>
+      </c>
+      <c r="J15" t="b">
+        <v>1</v>
       </c>
       <c r="K15" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L15" t="n">
         <v>2325015.737773068</v>
       </c>
-      <c r="L15" t="n">
+      <c r="M15" t="n">
         <v>0.8534101373010432</v>
       </c>
-      <c r="M15" t="n">
+      <c r="N15" t="n">
         <v>105.4608381877317</v>
       </c>
     </row>
@@ -1124,19 +1171,22 @@
       <c r="H16" t="n">
         <v>20</v>
       </c>
-      <c r="I16" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" t="n">
-        <v>66666.66666666667</v>
+      <c r="I16" t="n">
+        <v>79839608</v>
+      </c>
+      <c r="J16" t="b">
+        <v>1</v>
       </c>
       <c r="K16" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L16" t="n">
         <v>2285064.333602175</v>
       </c>
-      <c r="L16" t="n">
+      <c r="M16" t="n">
         <v>0.8683309134111425</v>
       </c>
-      <c r="M16" t="n">
+      <c r="N16" t="n">
         <v>309.3117198202964</v>
       </c>
     </row>
@@ -1167,19 +1217,22 @@
       <c r="H17" t="n">
         <v>0</v>
       </c>
-      <c r="I17" t="b">
+      <c r="I17" t="n">
+        <v>79557496</v>
+      </c>
+      <c r="J17" t="b">
         <v>0</v>
       </c>
-      <c r="J17" t="n">
-        <v>66666.66666666667</v>
-      </c>
       <c r="K17" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L17" t="n">
         <v>2365454.555998237</v>
       </c>
-      <c r="L17" t="n">
+      <c r="M17" t="n">
         <v>0.8388205957998875</v>
       </c>
-      <c r="M17" t="n">
+      <c r="N17" t="n">
         <v>669.5606121140974</v>
       </c>
     </row>
@@ -1210,19 +1263,22 @@
       <c r="H18" t="n">
         <v>20</v>
       </c>
-      <c r="I18" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" t="n">
-        <v>66666.66666666667</v>
+      <c r="I18" t="n">
+        <v>79693688</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
       </c>
       <c r="K18" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L18" t="n">
         <v>2242497.398426694</v>
       </c>
-      <c r="L18" t="n">
+      <c r="M18" t="n">
         <v>0.8848135125561716</v>
       </c>
-      <c r="M18" t="n">
+      <c r="N18" t="n">
         <v>189.439107813715</v>
       </c>
     </row>
@@ -1253,19 +1309,22 @@
       <c r="H19" t="n">
         <v>20</v>
       </c>
-      <c r="I19" t="b">
-        <v>1</v>
-      </c>
-      <c r="J19" t="n">
-        <v>66666.66666666667</v>
+      <c r="I19" t="n">
+        <v>80373112</v>
+      </c>
+      <c r="J19" t="b">
+        <v>1</v>
       </c>
       <c r="K19" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L19" t="n">
         <v>2316930.594991126</v>
       </c>
-      <c r="L19" t="n">
+      <c r="M19" t="n">
         <v>0.8563881906042161</v>
       </c>
-      <c r="M19" t="n">
+      <c r="N19" t="n">
         <v>203.4962240158126</v>
       </c>
     </row>
@@ -1296,19 +1355,22 @@
       <c r="H20" t="n">
         <v>0</v>
       </c>
-      <c r="I20" t="b">
+      <c r="I20" t="n">
+        <v>79640440</v>
+      </c>
+      <c r="J20" t="b">
         <v>0</v>
       </c>
-      <c r="J20" t="n">
-        <v>66666.66666666667</v>
-      </c>
       <c r="K20" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L20" t="n">
         <v>2339464.239480994</v>
       </c>
-      <c r="L20" t="n">
+      <c r="M20" t="n">
         <v>0.8481394870306672</v>
       </c>
-      <c r="M20" t="n">
+      <c r="N20" t="n">
         <v>854.6332258107595</v>
       </c>
     </row>
@@ -1339,19 +1401,22 @@
       <c r="H21" t="n">
         <v>20</v>
       </c>
-      <c r="I21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" t="n">
-        <v>66666.66666666667</v>
+      <c r="I21" t="n">
+        <v>79803768</v>
+      </c>
+      <c r="J21" t="b">
+        <v>1</v>
       </c>
       <c r="K21" t="n">
+        <v>66666.66666666667</v>
+      </c>
+      <c r="L21" t="n">
         <v>2278757.193923877</v>
       </c>
-      <c r="L21" t="n">
+      <c r="M21" t="n">
         <v>0.8707342780049971</v>
       </c>
-      <c r="M21" t="n">
+      <c r="N21" t="n">
         <v>78.63582322401209</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2023-05-13 Eligible for Experiment
</commit_message>
<xml_diff>
--- a/output/fit_clients/fit_round_1.xlsx
+++ b/output/fit_clients/fit_round_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,30 +471,25 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>mu</t>
+          <t>isSelected</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>isSelected</t>
+          <t>bandwidth</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>bandwidth</t>
+          <t>transRate</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>transRate</t>
+          <t>uploadTime</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>uploadTime</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>totalTime</t>
         </is>
@@ -510,40 +505,37 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>948.6258351773424</v>
+        <v>70.95848971701832</v>
       </c>
       <c r="D2" t="n">
-        <v>79684984</v>
+        <v>79561592</v>
       </c>
       <c r="E2" t="n">
-        <v>777439984.1132922</v>
+        <v>1126927007.043005</v>
       </c>
       <c r="F2" t="n">
-        <v>2.079986689209623</v>
+        <v>0.004220205241383404</v>
       </c>
       <c r="G2" t="n">
-        <v>486.1547903553521</v>
+        <v>25.04851854875356</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>79684984</v>
-      </c>
-      <c r="J2" t="b">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K2" t="n">
-        <v>66666.66666666667</v>
+        <v>109736.707696296</v>
       </c>
       <c r="L2" t="n">
-        <v>2285057.016324704</v>
+        <v>18.08138809386727</v>
       </c>
       <c r="M2" t="n">
-        <v>0.8683336940061932</v>
-      </c>
-      <c r="N2" t="n">
-        <v>487.0231240493583</v>
+        <v>43.12990664262082</v>
       </c>
     </row>
     <row r="3">
@@ -556,40 +548,37 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>213.5084900557135</v>
+        <v>175.9556230791904</v>
       </c>
       <c r="D3" t="n">
-        <v>79871352</v>
+        <v>79873912</v>
       </c>
       <c r="E3" t="n">
-        <v>1113552653.597529</v>
+        <v>232371787.401807</v>
       </c>
       <c r="F3" t="n">
-        <v>3.99530175271218</v>
+        <v>0.003491682868916071</v>
       </c>
       <c r="G3" t="n">
-        <v>76.57119629294125</v>
+        <v>302.4089996224546</v>
       </c>
       <c r="H3" t="n">
-        <v>20</v>
-      </c>
-      <c r="I3" t="n">
-        <v>79871352</v>
-      </c>
-      <c r="J3" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K3" t="n">
-        <v>66666.66666666667</v>
+        <v>97002.55162876946</v>
       </c>
       <c r="L3" t="n">
-        <v>2347839.027896418</v>
+        <v>20.45504954955761</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8451141566454695</v>
-      </c>
-      <c r="N3" t="n">
-        <v>77.41631044958672</v>
+        <v>322.8640491720122</v>
       </c>
     </row>
     <row r="4">
@@ -602,40 +591,37 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>437.7289654771055</v>
+        <v>118.5748232692446</v>
       </c>
       <c r="D4" t="n">
-        <v>79786872</v>
+        <v>79817080</v>
       </c>
       <c r="E4" t="n">
-        <v>1006415221.399078</v>
+        <v>1099128883.62274</v>
       </c>
       <c r="F4" t="n">
-        <v>4.370703740963037</v>
+        <v>0.003200154175598993</v>
       </c>
       <c r="G4" t="n">
-        <v>173.5120067573247</v>
+        <v>43.0536231732567</v>
       </c>
       <c r="H4" t="n">
         <v>20</v>
       </c>
-      <c r="I4" t="n">
-        <v>79786872</v>
-      </c>
-      <c r="J4" t="b">
-        <v>1</v>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K4" t="n">
-        <v>66666.66666666667</v>
+        <v>91467.14202951529</v>
       </c>
       <c r="L4" t="n">
-        <v>2356476.436018003</v>
+        <v>21.69294848372683</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8420164826060843</v>
-      </c>
-      <c r="N4" t="n">
-        <v>174.3540232399308</v>
+        <v>64.74657165698353</v>
       </c>
     </row>
     <row r="5">
@@ -648,40 +634,37 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>157.7329428977101</v>
+        <v>80.7821316518251</v>
       </c>
       <c r="D5" t="n">
-        <v>79050104</v>
+        <v>79235960</v>
       </c>
       <c r="E5" t="n">
-        <v>926520325.2614211</v>
+        <v>833180992.2729816</v>
       </c>
       <c r="F5" t="n">
-        <v>1.635689152173448</v>
+        <v>0.0029241020420135</v>
       </c>
       <c r="G5" t="n">
-        <v>67.28835407238329</v>
+        <v>38.41212060549256</v>
       </c>
       <c r="H5" t="n">
         <v>20</v>
       </c>
-      <c r="I5" t="n">
-        <v>79050104</v>
-      </c>
-      <c r="J5" t="b">
-        <v>1</v>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K5" t="n">
-        <v>66666.66666666667</v>
+        <v>85958.17114104528</v>
       </c>
       <c r="L5" t="n">
-        <v>2261945.303482444</v>
+        <v>23.08322726811183</v>
       </c>
       <c r="M5" t="n">
-        <v>0.8772060035869031</v>
-      </c>
-      <c r="N5" t="n">
-        <v>68.16556007597019</v>
+        <v>61.49534787360439</v>
       </c>
     </row>
     <row r="6">
@@ -694,40 +677,37 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>567.658788936207</v>
+        <v>80.74375796642178</v>
       </c>
       <c r="D6" t="n">
-        <v>79858040</v>
+        <v>79761784</v>
       </c>
       <c r="E6" t="n">
-        <v>902907777.7292607</v>
+        <v>895042835.8966057</v>
       </c>
       <c r="F6" t="n">
-        <v>4.596261683574578</v>
+        <v>0.00430839303353433</v>
       </c>
       <c r="G6" t="n">
-        <v>251.0340446242791</v>
+        <v>35.97741875568727</v>
       </c>
       <c r="H6" t="n">
         <v>20</v>
       </c>
-      <c r="I6" t="n">
-        <v>79858040</v>
-      </c>
-      <c r="J6" t="b">
-        <v>1</v>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K6" t="n">
-        <v>66666.66666666667</v>
+        <v>111183.5560113591</v>
       </c>
       <c r="L6" t="n">
-        <v>2361316.125842037</v>
+        <v>17.84609227462814</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8402907083406481</v>
-      </c>
-      <c r="N6" t="n">
-        <v>251.8743353326198</v>
+        <v>53.8235110303154</v>
       </c>
     </row>
     <row r="7">
@@ -740,40 +720,37 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>214.2700635860639</v>
+        <v>111.7396685830363</v>
       </c>
       <c r="D7" t="n">
-        <v>79890808</v>
+        <v>80025976</v>
       </c>
       <c r="E7" t="n">
-        <v>214294624.1260078</v>
+        <v>1405892873.14731</v>
       </c>
       <c r="F7" t="n">
-        <v>1.956763418070329</v>
+        <v>0.002292505142216274</v>
       </c>
       <c r="G7" t="n">
-        <v>399.4082581380183</v>
+        <v>31.80212449706709</v>
       </c>
       <c r="H7" t="n">
-        <v>10</v>
-      </c>
-      <c r="I7" t="n">
-        <v>79890808</v>
-      </c>
-      <c r="J7" t="b">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K7" t="n">
-        <v>66666.66666666667</v>
+        <v>72219.37576738487</v>
       </c>
       <c r="L7" t="n">
-        <v>2279183.352454564</v>
+        <v>27.47451053012403</v>
       </c>
       <c r="M7" t="n">
-        <v>0.8705714693217317</v>
-      </c>
-      <c r="N7" t="n">
-        <v>400.27882960734</v>
+        <v>59.27663502719112</v>
       </c>
     </row>
     <row r="8">
@@ -786,40 +763,37 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>896.6386415404207</v>
+        <v>123.9098299632842</v>
       </c>
       <c r="D8" t="n">
-        <v>80089464</v>
+        <v>79814520</v>
       </c>
       <c r="E8" t="n">
-        <v>479263710.0210323</v>
+        <v>1235208275.756846</v>
       </c>
       <c r="F8" t="n">
-        <v>2.129901950499447</v>
+        <v>0.0009087328629546882</v>
       </c>
       <c r="G8" t="n">
-        <v>749.1836613240447</v>
+        <v>40.03293936701237</v>
       </c>
       <c r="H8" t="n">
+        <v>9</v>
+      </c>
+      <c r="I8" t="b">
         <v>0</v>
       </c>
-      <c r="I8" t="n">
-        <v>80089464</v>
-      </c>
-      <c r="J8" t="b">
-        <v>0</v>
+      <c r="J8" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K8" t="n">
-        <v>66666.66666666667</v>
+        <v>34408.26517493059</v>
       </c>
       <c r="L8" t="n">
-        <v>2287337.864454519</v>
+        <v>57.66614474494507</v>
       </c>
       <c r="M8" t="n">
-        <v>0.8674678239863735</v>
-      </c>
-      <c r="N8" t="n">
-        <v>750.051129148031</v>
+        <v>97.69908411195745</v>
       </c>
     </row>
     <row r="9">
@@ -832,40 +806,37 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>528.3910167296074</v>
+        <v>110.2705246966666</v>
       </c>
       <c r="D9" t="n">
-        <v>79675768</v>
+        <v>79492984</v>
       </c>
       <c r="E9" t="n">
-        <v>803017733.3737501</v>
+        <v>967188858.4782858</v>
       </c>
       <c r="F9" t="n">
-        <v>4.166466358017141</v>
+        <v>0.002054846491575216</v>
       </c>
       <c r="G9" t="n">
-        <v>262.1359299585832</v>
+        <v>45.31551919019817</v>
       </c>
       <c r="H9" t="n">
-        <v>20</v>
-      </c>
-      <c r="I9" t="n">
-        <v>79675768</v>
-      </c>
-      <c r="J9" t="b">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K9" t="n">
-        <v>66666.66666666667</v>
+        <v>66574.94907215168</v>
       </c>
       <c r="L9" t="n">
-        <v>2351873.685337585</v>
+        <v>29.80388310698668</v>
       </c>
       <c r="M9" t="n">
-        <v>0.8436643567935459</v>
-      </c>
-      <c r="N9" t="n">
-        <v>262.9795943153767</v>
+        <v>75.11940229718485</v>
       </c>
     </row>
     <row r="10">
@@ -878,40 +849,37 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>230.6254062478076</v>
+        <v>109.2942173926688</v>
       </c>
       <c r="D10" t="n">
-        <v>80101240</v>
+        <v>80046456</v>
       </c>
       <c r="E10" t="n">
-        <v>644337456.96216</v>
+        <v>1828838693.402923</v>
       </c>
       <c r="F10" t="n">
-        <v>4.221320616045391</v>
+        <v>0.002065237360215993</v>
       </c>
       <c r="G10" t="n">
-        <v>143.3517547082322</v>
+        <v>23.91849755567599</v>
       </c>
       <c r="H10" t="n">
         <v>20</v>
       </c>
-      <c r="I10" t="n">
-        <v>80101240</v>
-      </c>
-      <c r="J10" t="b">
-        <v>1</v>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K10" t="n">
-        <v>66666.66666666667</v>
+        <v>66827.82902013171</v>
       </c>
       <c r="L10" t="n">
-        <v>2353131.690490548</v>
+        <v>29.69110367781463</v>
       </c>
       <c r="M10" t="n">
-        <v>0.8432133263167957</v>
-      </c>
-      <c r="N10" t="n">
-        <v>144.194968034549</v>
+        <v>53.60960123349062</v>
       </c>
     </row>
     <row r="11">
@@ -924,40 +892,37 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>675.3629726446641</v>
+        <v>153.218164522722</v>
       </c>
       <c r="D11" t="n">
-        <v>79580024</v>
+        <v>79497592</v>
       </c>
       <c r="E11" t="n">
-        <v>1260029743.479902</v>
+        <v>788234814.5322708</v>
       </c>
       <c r="F11" t="n">
-        <v>1.121991114536063</v>
+        <v>0.002172038545255918</v>
       </c>
       <c r="G11" t="n">
-        <v>213.2703686158301</v>
+        <v>77.26425492538016</v>
       </c>
       <c r="H11" t="n">
-        <v>20</v>
-      </c>
-      <c r="I11" t="n">
-        <v>79580024</v>
-      </c>
-      <c r="J11" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K11" t="n">
-        <v>66666.66666666667</v>
+        <v>69394.16014641368</v>
       </c>
       <c r="L11" t="n">
-        <v>2225689.479983788</v>
+        <v>28.59306886650957</v>
       </c>
       <c r="M11" t="n">
-        <v>0.8914954299979225</v>
-      </c>
-      <c r="N11" t="n">
-        <v>214.161864045828</v>
+        <v>105.8573237918897</v>
       </c>
     </row>
     <row r="12">
@@ -970,40 +935,37 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>847.9483284738407</v>
+        <v>52.69345785456528</v>
       </c>
       <c r="D12" t="n">
-        <v>79984504</v>
+        <v>79762808</v>
       </c>
       <c r="E12" t="n">
-        <v>1743888542.711137</v>
+        <v>1304380947.56723</v>
       </c>
       <c r="F12" t="n">
-        <v>2.469650462425335</v>
+        <v>0.003557886963972279</v>
       </c>
       <c r="G12" t="n">
-        <v>194.4583177465247</v>
+        <v>16.11100717757591</v>
       </c>
       <c r="H12" t="n">
         <v>20</v>
       </c>
-      <c r="I12" t="n">
-        <v>79984504</v>
-      </c>
-      <c r="J12" t="b">
-        <v>1</v>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K12" t="n">
-        <v>66666.66666666667</v>
+        <v>98222.0433687905</v>
       </c>
       <c r="L12" t="n">
-        <v>2301572.521061347</v>
+        <v>20.20108655803495</v>
       </c>
       <c r="M12" t="n">
-        <v>0.8621027501166939</v>
-      </c>
-      <c r="N12" t="n">
-        <v>195.3204204966414</v>
+        <v>36.31209373561087</v>
       </c>
     </row>
     <row r="13">
@@ -1016,40 +978,37 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>209.8112744772966</v>
+        <v>185.9418346898805</v>
       </c>
       <c r="D13" t="n">
-        <v>79686520</v>
+        <v>80041848</v>
       </c>
       <c r="E13" t="n">
-        <v>604644162.542438</v>
+        <v>983761988.3588175</v>
       </c>
       <c r="F13" t="n">
-        <v>3.297803663411722</v>
+        <v>0.002715096879788233</v>
       </c>
       <c r="G13" t="n">
-        <v>138.2559475110051</v>
+        <v>75.64394764793487</v>
       </c>
       <c r="H13" t="n">
-        <v>20</v>
-      </c>
-      <c r="I13" t="n">
-        <v>79686520</v>
-      </c>
-      <c r="J13" t="b">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K13" t="n">
-        <v>66666.66666666667</v>
+        <v>81597.38144287353</v>
       </c>
       <c r="L13" t="n">
-        <v>2329385.763906141</v>
+        <v>24.31685876328196</v>
       </c>
       <c r="M13" t="n">
-        <v>0.8518091038183018</v>
-      </c>
-      <c r="N13" t="n">
-        <v>139.1077566148234</v>
+        <v>99.96080641121682</v>
       </c>
     </row>
     <row r="14">
@@ -1062,40 +1021,37 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>842.2294025010319</v>
+        <v>197.075549015551</v>
       </c>
       <c r="D14" t="n">
-        <v>79952248</v>
+        <v>79997816</v>
       </c>
       <c r="E14" t="n">
-        <v>1923816633.366146</v>
+        <v>1645456896.429853</v>
       </c>
       <c r="F14" t="n">
-        <v>1.755381922456259</v>
+        <v>0.001254936285397894</v>
       </c>
       <c r="G14" t="n">
-        <v>175.0118303734365</v>
+        <v>47.90649193683429</v>
       </c>
       <c r="H14" t="n">
-        <v>20</v>
-      </c>
-      <c r="I14" t="n">
-        <v>79952248</v>
-      </c>
-      <c r="J14" t="b">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K14" t="n">
-        <v>66666.66666666667</v>
+        <v>45143.10254511117</v>
       </c>
       <c r="L14" t="n">
-        <v>2268737.726939628</v>
+        <v>43.95338131705085</v>
       </c>
       <c r="M14" t="n">
-        <v>0.8745797173640425</v>
-      </c>
-      <c r="N14" t="n">
-        <v>175.8864100908005</v>
+        <v>91.85987325388514</v>
       </c>
     </row>
     <row r="15">
@@ -1108,40 +1064,37 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>156.0108260587542</v>
+        <v>72.50100601321395</v>
       </c>
       <c r="D15" t="n">
-        <v>79846264</v>
+        <v>79731064</v>
       </c>
       <c r="E15" t="n">
-        <v>595410949.1316419</v>
+        <v>1371947743.31511</v>
       </c>
       <c r="F15" t="n">
-        <v>3.151317505008611</v>
+        <v>0.003943618243461979</v>
       </c>
       <c r="G15" t="n">
-        <v>104.6074280504306</v>
+        <v>21.06706461186349</v>
       </c>
       <c r="H15" t="n">
         <v>20</v>
       </c>
-      <c r="I15" t="n">
-        <v>79846264</v>
-      </c>
-      <c r="J15" t="b">
-        <v>1</v>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K15" t="n">
-        <v>66666.66666666667</v>
+        <v>105072.5329416696</v>
       </c>
       <c r="L15" t="n">
-        <v>2325015.737773068</v>
+        <v>18.88402177476308</v>
       </c>
       <c r="M15" t="n">
-        <v>0.8534101373010432</v>
-      </c>
-      <c r="N15" t="n">
-        <v>105.4608381877317</v>
+        <v>39.95108638662657</v>
       </c>
     </row>
     <row r="16">
@@ -1154,40 +1107,37 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>405.6857339024511</v>
+        <v>96.3739219971601</v>
       </c>
       <c r="D16" t="n">
-        <v>79839608</v>
+        <v>79832952</v>
       </c>
       <c r="E16" t="n">
-        <v>525052426.6503575</v>
+        <v>789119212.298843</v>
       </c>
       <c r="F16" t="n">
-        <v>2.080144939064407</v>
+        <v>0.002360910960038808</v>
       </c>
       <c r="G16" t="n">
-        <v>308.4433889068852</v>
+        <v>48.74938139218275</v>
       </c>
       <c r="H16" t="n">
-        <v>20</v>
-      </c>
-      <c r="I16" t="n">
-        <v>79839608</v>
-      </c>
-      <c r="J16" t="b">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K16" t="n">
-        <v>66666.66666666667</v>
+        <v>73792.20098831299</v>
       </c>
       <c r="L16" t="n">
-        <v>2285064.333602175</v>
+        <v>26.88891201814472</v>
       </c>
       <c r="M16" t="n">
-        <v>0.8683309134111425</v>
-      </c>
-      <c r="N16" t="n">
-        <v>309.3117198202964</v>
+        <v>75.63829341032746</v>
       </c>
     </row>
     <row r="17">
@@ -1200,40 +1150,37 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>570.3085645938759</v>
+        <v>132.3194100858378</v>
       </c>
       <c r="D17" t="n">
-        <v>79557496</v>
+        <v>79816568</v>
       </c>
       <c r="E17" t="n">
-        <v>339246618.8624388</v>
+        <v>1734880216.672365</v>
       </c>
       <c r="F17" t="n">
-        <v>4.798346663772044</v>
+        <v>0.003627136141331431</v>
       </c>
       <c r="G17" t="n">
-        <v>668.7217915182974</v>
+        <v>30.4380702809947</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" t="n">
-        <v>79557496</v>
-      </c>
-      <c r="J17" t="b">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K17" t="n">
-        <v>66666.66666666667</v>
+        <v>99483.44712401924</v>
       </c>
       <c r="L17" t="n">
-        <v>2365454.555998237</v>
+        <v>19.94494619317365</v>
       </c>
       <c r="M17" t="n">
-        <v>0.8388205957998875</v>
-      </c>
-      <c r="N17" t="n">
-        <v>669.5606121140974</v>
+        <v>50.38301647416836</v>
       </c>
     </row>
     <row r="18">
@@ -1246,40 +1193,37 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>135.4339272273684</v>
+        <v>176.1311528522601</v>
       </c>
       <c r="D18" t="n">
-        <v>79693688</v>
+        <v>79846264</v>
       </c>
       <c r="E18" t="n">
-        <v>286210112.081395</v>
+        <v>1118402169.629412</v>
       </c>
       <c r="F18" t="n">
-        <v>1.336240811461762</v>
+        <v>0.004926720339789661</v>
       </c>
       <c r="G18" t="n">
-        <v>188.5542943011588</v>
+        <v>62.87279706335826</v>
       </c>
       <c r="H18" t="n">
-        <v>20</v>
-      </c>
-      <c r="I18" t="n">
-        <v>79693688</v>
-      </c>
-      <c r="J18" t="b">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K18" t="n">
-        <v>66666.66666666667</v>
+        <v>120830.5506456392</v>
       </c>
       <c r="L18" t="n">
-        <v>2242497.398426694</v>
+        <v>16.42127747823526</v>
       </c>
       <c r="M18" t="n">
-        <v>0.8848135125561716</v>
-      </c>
-      <c r="N18" t="n">
-        <v>189.439107813715</v>
+        <v>79.29407454159352</v>
       </c>
     </row>
     <row r="19">
@@ -1292,40 +1236,37 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>381.0173787623345</v>
+        <v>102.2661244817619</v>
       </c>
       <c r="D19" t="n">
-        <v>80373112</v>
+        <v>79854968</v>
       </c>
       <c r="E19" t="n">
-        <v>755615309.6083876</v>
+        <v>1541271038.75871</v>
       </c>
       <c r="F19" t="n">
-        <v>2.897237544344244</v>
+        <v>0.004131978223816866</v>
       </c>
       <c r="G19" t="n">
-        <v>202.6398358252084</v>
+        <v>26.49260867365715</v>
       </c>
       <c r="H19" t="n">
         <v>20</v>
       </c>
-      <c r="I19" t="n">
-        <v>80373112</v>
-      </c>
-      <c r="J19" t="b">
-        <v>1</v>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K19" t="n">
-        <v>66666.66666666667</v>
+        <v>108270.0903728412</v>
       </c>
       <c r="L19" t="n">
-        <v>2316930.594991126</v>
+        <v>18.32631702039958</v>
       </c>
       <c r="M19" t="n">
-        <v>0.8563881906042161</v>
-      </c>
-      <c r="N19" t="n">
-        <v>203.4962240158126</v>
+        <v>44.81892569405673</v>
       </c>
     </row>
     <row r="20">
@@ -1338,40 +1279,37 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>405.4509258528423</v>
+        <v>165.4740402215803</v>
       </c>
       <c r="D20" t="n">
-        <v>79640440</v>
+        <v>80000888</v>
       </c>
       <c r="E20" t="n">
-        <v>189100809.1530675</v>
+        <v>1386432394.135247</v>
       </c>
       <c r="F20" t="n">
-        <v>3.662129080582477</v>
+        <v>0.002262925582568383</v>
       </c>
       <c r="G20" t="n">
-        <v>853.7850863237288</v>
+        <v>47.74149181262842</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" t="n">
-        <v>79640440</v>
-      </c>
-      <c r="J20" t="b">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K20" t="n">
-        <v>66666.66666666667</v>
+        <v>71532.30099033478</v>
       </c>
       <c r="L20" t="n">
-        <v>2339464.239480994</v>
+        <v>27.73840590236427</v>
       </c>
       <c r="M20" t="n">
-        <v>0.8481394870306672</v>
-      </c>
-      <c r="N20" t="n">
-        <v>854.6332258107595</v>
+        <v>75.47989771499269</v>
       </c>
     </row>
     <row r="21">
@@ -1384,40 +1322,37 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>331.3686920797364</v>
+        <v>71.22950717745928</v>
       </c>
       <c r="D21" t="n">
-        <v>79803768</v>
+        <v>80230776</v>
       </c>
       <c r="E21" t="n">
-        <v>1700279044.466556</v>
+        <v>427332063.0859565</v>
       </c>
       <c r="F21" t="n">
-        <v>1.94811245548718</v>
+        <v>0.003963270018734173</v>
       </c>
       <c r="G21" t="n">
-        <v>77.76508894600708</v>
+        <v>66.86601742069158</v>
       </c>
       <c r="H21" t="n">
-        <v>20</v>
-      </c>
-      <c r="I21" t="n">
-        <v>79803768</v>
-      </c>
-      <c r="J21" t="b">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>76923.07692307692</v>
       </c>
       <c r="K21" t="n">
-        <v>66666.66666666667</v>
+        <v>105410.4746201164</v>
       </c>
       <c r="L21" t="n">
-        <v>2278757.193923877</v>
+        <v>18.82348037185803</v>
       </c>
       <c r="M21" t="n">
-        <v>0.8707342780049971</v>
-      </c>
-      <c r="N21" t="n">
-        <v>78.63582322401209</v>
+        <v>85.6894977925496</v>
       </c>
     </row>
   </sheetData>

</xml_diff>